<commit_message>
add first adaptation experiment
</commit_message>
<xml_diff>
--- a/experimental-design/stimuli-brainstorming.xlsx
+++ b/experimental-design/stimuli-brainstorming.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="2780" yWindow="460" windowWidth="28040" windowHeight="16580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>the coffee is cold</t>
   </si>
@@ -176,7 +176,16 @@
     <t>there is cream in the chocolate</t>
   </si>
   <si>
-    <t>your friend has a box of chocolate. She knows that the round ones are filled with cream.</t>
+    <t>your friend has a box of chocolate. She knows that the round ones are filled with cream. She hands you a piece.</t>
+  </si>
+  <si>
+    <t>your friend has a box of with chocolates. She knows that 8 or 9 of the 10 have cream in them but she can’t tell from looking at them which ones are which. She hands you a piece.</t>
+  </si>
+  <si>
+    <t>your friend has a box of with chocolates. She knows that 5 or 6 of the 10 have cream in them but she can’t tell from looking at them which ones are which. She hands you a piece.</t>
+  </si>
+  <si>
+    <t>your friend has a box of with chocolates. She thinks that one of them is filled with cream but she can’t tell from looking at them which one it is. She hands you a piece.</t>
   </si>
 </sst>
 </file>
@@ -542,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -813,16 +822,22 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>49</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="C24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>